<commit_message>
removed omgekeerd spuien 30 maart 2022 18:00
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4458" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="65">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L276"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="H268" sqref="H268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6857,9 +6857,7 @@
       <c r="G266" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H266" s="29" t="s">
-        <v>48</v>
-      </c>
+      <c r="H266" s="29"/>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A267" s="23">
@@ -29252,7 +29250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
in sheet march 2023 there was a february date that should have been a march date: changed 3 feb to 3 march
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="H268" sqref="H268"/>
+    <sheetView topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="H266" sqref="H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17052,8 +17052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17391,7 +17391,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
-        <v>44960</v>
+        <v>44988</v>
       </c>
       <c r="B18" s="24">
         <v>3.125E-2</v>

</xml_diff>

<commit_message>
25 april 2023 6:35 was designated as "omgekeerd spuibeheer" but should have been "einde omgekeerd spuibeheer": corrected
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -17052,7 +17052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -23255,8 +23255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="H229" sqref="H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28324,7 +28324,7 @@
         <v>13</v>
       </c>
       <c r="H229" s="51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
removed "einde omgekeerd spuibeheer" at 3 april 2023
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="65">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -23255,8 +23255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="H229" sqref="H229"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23794,9 +23794,7 @@
       <c r="G26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>15</v>
-      </c>
+      <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>

</xml_diff>

<commit_message>
4/4/2022 12:28 should probably be 2:28: changed
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -13289,8 +13289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="G164" sqref="G164"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14061,7 +14061,7 @@
         <v>44685</v>
       </c>
       <c r="B37" s="24">
-        <v>2.52</v>
+        <v>2.1033333333333335</v>
       </c>
       <c r="C37" s="25">
         <v>2.13</v>
@@ -23255,8 +23255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
19 maart had 1 rij hoger moeten staan (161->160) thv tijdstip 1h10: aangepast
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -13289,8 +13289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17052,8 +17052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20541,7 +20541,9 @@
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A160" s="23"/>
+      <c r="A160" s="23">
+        <v>45004</v>
+      </c>
       <c r="B160" s="24">
         <v>4.8611111111111112E-2</v>
       </c>
@@ -20563,9 +20565,6 @@
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A161" s="23">
-        <v>45004</v>
-      </c>
       <c r="B161" s="24">
         <v>0.16666666666666666</v>
       </c>

</xml_diff>

<commit_message>
20 april 2023 19h20 "einde omgekeerd spuibeheer" verwijdert
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4455" uniqueCount="65">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -17052,8 +17052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23254,8 +23254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="H185" sqref="H185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27338,9 +27338,7 @@
       <c r="G185" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H185" s="51" t="s">
-        <v>15</v>
-      </c>
+      <c r="H185" s="51"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="23">

</xml_diff>

<commit_message>
laatste rij april 2023 sheet moet naar mei 2023 sheet: verwijderd en einde omgekeerd spuibeheer aangevuld in volgende sheet
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4455" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="65">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -985,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L276"/>
   <sheetViews>
-    <sheetView topLeftCell="A247" workbookViewId="0">
+    <sheetView topLeftCell="A265" workbookViewId="0">
       <selection activeCell="H266" sqref="H266"/>
     </sheetView>
   </sheetViews>
@@ -23252,10 +23252,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L270"/>
+  <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="H185" sqref="H185"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="D266" sqref="D266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29208,30 +29208,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A270" s="23"/>
-      <c r="B270" s="24">
-        <v>6.9444444444444434E-2</v>
-      </c>
-      <c r="C270" s="25">
-        <v>2.7</v>
-      </c>
-      <c r="D270" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E270" s="27">
-        <v>2.7</v>
-      </c>
-      <c r="F270" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G270" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H270" s="51" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
@@ -29246,7 +29222,7 @@
   <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29364,7 +29340,9 @@
       <c r="G7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>

</xml_diff>

<commit_message>
in sheet mei 2023 moet 2 mei 1 rij hoger (15->14): aangepast
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -23254,7 +23254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+    <sheetView topLeftCell="A253" workbookViewId="0">
       <selection activeCell="D266" sqref="D266"/>
     </sheetView>
   </sheetViews>
@@ -29221,8 +29221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29479,7 +29479,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
+      <c r="A14" s="23">
+        <v>45048</v>
+      </c>
       <c r="B14" s="24">
         <v>0.1111111111111111</v>
       </c>
@@ -29503,9 +29505,6 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="23">
-        <v>45048</v>
-      </c>
       <c r="B15" s="24">
         <v>0.19097222222222221</v>
       </c>

</xml_diff>

<commit_message>
7 mei 2023 8h "einde omgekeerd spuibeheer" verwijdert
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4451" uniqueCount="65">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -29221,8 +29221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30551,9 +30551,7 @@
       <c r="G61" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H61" s="32" t="s">
-        <v>43</v>
-      </c>
+      <c r="H61" s="32"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="23"/>

</xml_diff>

<commit_message>
11 maart 2022 moest 1 rij hoger
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L276"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="H266" sqref="H266"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3093,7 +3093,9 @@
       <c r="H96" s="32"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="23"/>
+      <c r="A97" s="23">
+        <v>44631</v>
+      </c>
       <c r="B97" s="24">
         <v>0.15625</v>
       </c>
@@ -3117,9 +3119,6 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="23">
-        <v>44631</v>
-      </c>
       <c r="B98" s="24">
         <v>0.33333333333333331</v>
       </c>
@@ -29221,7 +29220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
23 april 2023 moest 2 rijen hoger: aangepast
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23253,8 +23253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="D266" sqref="D266"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27762,7 +27762,9 @@
       <c r="H204" s="51"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A205" s="23"/>
+      <c r="A205" s="23">
+        <v>45039</v>
+      </c>
       <c r="B205" s="24">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -27808,9 +27810,6 @@
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A207" s="23">
-        <v>45039</v>
-      </c>
       <c r="B207" s="24">
         <v>0.23958333333333334</v>
       </c>

</xml_diff>